<commit_message>
Reporte total y por tipo licencia
</commit_message>
<xml_diff>
--- a/totalidadLiencias.xlsx
+++ b/totalidadLiencias.xlsx
@@ -17,13 +17,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="000000FF"/>
+      <sz val="24"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <strike val="0"/>
+      <color rgb="00000000"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +60,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,165 +442,83 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Reporte totalidad licencias</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Fecha y hora de creación: 06/07/2021, 22:07:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Cédula</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Nombre completo</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Fecha Nacimiento</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Fecha Expedición</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Fecha Vencimiento</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Tipo licencia</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Tipo Sangre</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Donador</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Sede</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Puntaje</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>726221143</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Arthur Lopez Slama</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>11-1-1948</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>7-6-2021</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>7-6-2026</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Licencia D2</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>AB-</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Limón, Barrio Sandoval de Moín</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>746232283</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Coralie Masters Byron</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>29-6-1961</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7-6-2021</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>7-6-2026</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Licencia D1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>B-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Atlántico, Guápiles</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>328367517</v>
+        <v>726221143</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Joe Petrey Elzy</t>
+          <t>Arthur Lopez Slama</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16-7-1956</t>
+          <t>11-1-1948</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -595,12 +533,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Licencia E1</t>
+          <t>Licencia D2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>AB-</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -610,25 +548,25 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>GAM, Tránsito Cartago</t>
+          <t>Limón, Barrio Sandoval de Moín</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>522446971</v>
+        <v>746232283</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Kenneth Badman Martin</t>
+          <t>Coralie Masters Byron</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20-12-1950</t>
+          <t>29-6-1961</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -643,40 +581,40 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Licencia C2 (autobús)</t>
+          <t>Licencia D1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Pacífico, Liberia</t>
+          <t>Atlántico, Guápiles</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>621149563</v>
+        <v>328367517</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nedra Jones Barnes</t>
+          <t>Joe Petrey Elzy</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>14-2-1992</t>
+          <t>16-7-1956</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -691,12 +629,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Licencia B4 (camión articulado)</t>
+          <t>Licencia E1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>A-</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -706,25 +644,25 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Puntarenas, Chacarita</t>
+          <t>GAM, Tránsito Cartago</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>282956666</v>
+        <v>522446971</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mary Russell Carlton</t>
+          <t>Kenneth Badman Martin</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>14-2-1999</t>
+          <t>20-12-1950</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -734,45 +672,45 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>7-6-2024</t>
+          <t>7-6-2026</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Licencia B2 (camión pequeño)</t>
+          <t>Licencia C2 (autobús)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>AB-</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Zona Norte, San Carlos</t>
+          <t>Pacífico, Liberia</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>397787626</v>
+        <v>621149563</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Phyllis Johnson Oleson</t>
+          <t>Nedra Jones Barnes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>21-3-1996</t>
+          <t>14-2-1992</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -782,12 +720,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>7-6-2024</t>
+          <t>7-6-2026</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Licencia B2 (camión pequeño)</t>
+          <t>Licencia B4 (camión articulado)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -797,30 +735,30 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>GAM, Tránsito Cartago</t>
+          <t>Puntarenas, Chacarita</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>856839446</v>
+        <v>282956666</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Laurie Derego Champagne</t>
+          <t>Mary Russell Carlton</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6-3-1992</t>
+          <t>14-2-1999</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -830,45 +768,45 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>7-6-2026</t>
+          <t>7-6-2024</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Licencia C2 (autobús)</t>
+          <t>Licencia B2 (camión pequeño)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>O-</t>
+          <t>AB-</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Zona Sur, Perez Zeledón</t>
+          <t>Zona Norte, San Carlos</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>315151228</v>
+        <v>397787626</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Amelia Mahon Gabriel</t>
+          <t>Phyllis Johnson Oleson</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12-5-1979</t>
+          <t>21-3-1996</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -878,22 +816,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>7-6-2026</t>
+          <t>7-6-2024</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Licencia D2</t>
+          <t>Licencia B2 (camión pequeño)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -902,21 +840,21 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>531523163</v>
+        <v>856839446</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alice Brady Valenziano</t>
+          <t>Laurie Derego Champagne</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>10-8-1997</t>
+          <t>6-3-1992</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -926,45 +864,45 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>7-6-2024</t>
+          <t>7-6-2026</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Licencia D3</t>
+          <t>Licencia C2 (autobús)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>O-</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Pacífico, Liberia</t>
+          <t>Zona Sur, Perez Zeledón</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>374188785</v>
+        <v>315151228</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Andrew Regan Brown</t>
+          <t>Amelia Mahon Gabriel</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>12-2-2002</t>
+          <t>12-5-1979</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -974,17 +912,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>7-6-2024</t>
+          <t>7-6-2026</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Licencia B1</t>
+          <t>Licencia D2</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>AB+</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -998,21 +936,21 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>394393882</v>
+        <v>531523163</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lisa Stoll Steffen</t>
+          <t>Alice Brady Valenziano</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>22-9-1985</t>
+          <t>10-8-1997</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1022,45 +960,45 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>7-6-2026</t>
+          <t>7-6-2024</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Licencia B3 (camión pesado)</t>
+          <t>Licencia D3</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>O-</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>GAM, Tránsito Cartago</t>
+          <t>Pacífico, Liberia</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>772126671</v>
+        <v>374188785</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jimmy Hatton Rivet</t>
+          <t>Andrew Regan Brown</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6-8-1996</t>
+          <t>12-2-2002</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1075,12 +1013,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Licencia E1</t>
+          <t>Licencia B1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>AB-</t>
+          <t>AB+</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1090,25 +1028,25 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Limón, Barrio Sandoval de Moín</t>
+          <t>GAM, Tránsito Cartago</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>943679397</v>
+        <v>394393882</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>David Rocha Price</t>
+          <t>Lisa Stoll Steffen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>15-12-1978</t>
+          <t>22-9-1985</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1123,40 +1061,40 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Licencia B1</t>
+          <t>Licencia B3 (camión pesado)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>AB-</t>
+          <t>O-</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Zona Sur, Perez Zeledón</t>
+          <t>GAM, Tránsito Cartago</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>633358587</v>
+        <v>772126671</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Francesca Meierhofer Kyles</t>
+          <t>Jimmy Hatton Rivet</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6-3-1981</t>
+          <t>6-8-1996</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1166,12 +1104,12 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>7-6-2026</t>
+          <t>7-6-2024</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Licencia A2</t>
+          <t>Licencia E1</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1186,25 +1124,25 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Zona Sur, Río Claro de Golfito</t>
+          <t>Limón, Barrio Sandoval de Moín</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>292271584</v>
+        <v>943679397</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Sandra Campbell Denning</t>
+          <t>David Rocha Price</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7-1-1962</t>
+          <t>15-12-1978</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1219,40 +1157,40 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Licencia E1</t>
+          <t>Licencia B1</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>AB-</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Zona Norte, San Carlos</t>
+          <t>Zona Sur, Perez Zeledón</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>664222567</v>
+        <v>633358587</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Viola Rodriguez Robles</t>
+          <t>Francesca Meierhofer Kyles</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>22-4-1965</t>
+          <t>6-3-1981</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1267,12 +1205,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Licencia B2 (camión pequeño)</t>
+          <t>Licencia A2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>AB-</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1286,21 +1224,21 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>871481944</v>
+        <v>292271584</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Robert Vanblarcom Rauf</t>
+          <t>Sandra Campbell Denning</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>25-5-1973</t>
+          <t>7-1-1962</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1315,12 +1253,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Licencia C1 (taxi)</t>
+          <t>Licencia E1</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1330,25 +1268,25 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Sede Central, San Sebastián</t>
+          <t>Zona Norte, San Carlos</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>614436723</v>
+        <v>664222567</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Robert Francis Marks</t>
+          <t>Viola Rodriguez Robles</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>3-10-1954</t>
+          <t>22-4-1965</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1363,12 +1301,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Licencia D1</t>
+          <t>Licencia B2 (camión pequeño)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>A-</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1382,21 +1320,21 @@
         </is>
       </c>
       <c r="J20" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>235659655</v>
+        <v>871481944</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kathy Robinson Raines</t>
+          <t>Robert Vanblarcom Rauf</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>22-1-1961</t>
+          <t>25-5-1973</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1411,12 +1349,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Licencia D1</t>
+          <t>Licencia C1 (taxi)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>AB+</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1426,25 +1364,25 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>GAM, Tránsito San Ramón</t>
+          <t>Sede Central, San Sebastián</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>434959977</v>
+        <v>614436723</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lonnie Grasso Mayen</t>
+          <t>Robert Francis Marks</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>25-6-1967</t>
+          <t>3-10-1954</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1464,7 +1402,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>AB-</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1474,25 +1412,25 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>GAM, Barva de Heredia</t>
+          <t>Zona Sur, Río Claro de Golfito</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>763256373</v>
+        <v>235659655</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Carol Himenez Tucker</t>
+          <t>Kathy Robinson Raines</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6-6-1953</t>
+          <t>22-1-1961</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1507,40 +1445,40 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Licencia E2</t>
+          <t>Licencia D1</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>A+</t>
+          <t>AB+</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Si</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Limón, Barrio Sandoval de Moín</t>
+          <t>GAM, Tránsito San Ramón</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>926974132</v>
+        <v>434959977</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jennifer Delgadillo Oneil</t>
+          <t>Lonnie Grasso Mayen</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>26-10-1987</t>
+          <t>25-6-1967</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1555,12 +1493,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Licencia A1</t>
+          <t>Licencia D1</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>AB-</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1570,25 +1508,25 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Sede Central, San Sebastián</t>
+          <t>GAM, Barva de Heredia</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>564953861</v>
+        <v>763256373</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Douglas Mickens Chalmers</t>
+          <t>Carol Himenez Tucker</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1-1-1991</t>
+          <t>6-6-1953</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1603,22 +1541,22 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Licencia D3</t>
+          <t>Licencia E2</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>O-</t>
+          <t>A+</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Si</t>
+          <t>No</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Pacífico, Liberia</t>
+          <t>Limón, Barrio Sandoval de Moín</t>
         </is>
       </c>
       <c r="J25" t="n">
@@ -1627,16 +1565,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>358382829</v>
+        <v>926974132</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Charlie Stansberry Wainwright</t>
+          <t>Jennifer Delgadillo Oneil</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7-2-1985</t>
+          <t>26-10-1987</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1651,7 +1589,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Licencia D3</t>
+          <t>Licencia A1</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1666,14 +1604,114 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>GAM, Tránsito Cartago</t>
+          <t>Sede Central, San Sebastián</t>
         </is>
       </c>
       <c r="J26" t="n">
         <v>9</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>564953861</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Douglas Mickens Chalmers</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>1-1-1991</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>7-6-2021</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>7-6-2026</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Licencia D3</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>O-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Pacífico, Liberia</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>358382829</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Charlie Stansberry Wainwright</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>7-2-1985</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>7-6-2021</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>7-6-2026</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Licencia D3</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>GAM, Tránsito Cartago</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>